<commit_message>
excel ibo and customer user
</commit_message>
<xml_diff>
--- a/mkxProject/src/main/java/resorce/data.xlsx
+++ b/mkxProject/src/main/java/resorce/data.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ibo" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="customer" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastname</t>
+  </si>
   <si>
     <t xml:space="preserve">sponsor</t>
   </si>
@@ -31,10 +41,55 @@
     <t xml:space="preserve">confirmpassword</t>
   </si>
   <si>
-    <t xml:space="preserve">Mkx-business-admin</t>
+    <t xml:space="preserve">Enrollmentpackage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billing adress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mkx.epixel.link/en/register/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkx-business-admin</t>
   </si>
   <si>
     <t xml:space="preserve">As@12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkx-business-fee-pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">welsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirm password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mkx.epixel.link/en/customer-register/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raj</t>
   </si>
 </sst>
 </file>
@@ -44,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -65,6 +120,19 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monospace"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -110,8 +178,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -124,6 +208,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -132,21 +276,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="26.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.21"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -156,22 +304,76 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>635123</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="As@12345"/>
-    <hyperlink ref="C2" r:id="rId2" display="As@12345"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://mkx.epixel.link/en/register/"/>
+    <hyperlink ref="E2" r:id="rId2" display="As@12345"/>
+    <hyperlink ref="F2" r:id="rId3" display="As@12345"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -181,4 +383,81 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.12"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://mkx.epixel.link/en/customer-register/"/>
+    <hyperlink ref="E2" r:id="rId2" display="As@12345"/>
+    <hyperlink ref="F2" r:id="rId3" display="As@12345"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>